<commit_message>
First Commit , env independent login with url and credentials
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/smf.xlsx
+++ b/src/test/resources/testdata/smf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="87">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -37,15 +37,171 @@
     <t xml:space="preserve">status</t>
   </si>
   <si>
+    <t xml:space="preserve">DMNTOd7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EuGiOx7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aYAIx2R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pl0DFDw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9x0r5a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8BubxM9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puD4YmL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5NU9w8E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7WNdd8C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8gvq2JN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZCKEGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFEVT8s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptOj0zS Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xPocWW Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">352915305692302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">354150266351986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2duawu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhi1hlr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StaticPass@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reseller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ig26GfY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k8BytpD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reseller user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kx0h9PW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uCOwwTh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aiY9k5x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TKLddPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPL9tVN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5uqGbei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kp8Tw5Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retailer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JRxj2A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0HWR4LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">616lw2n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmdUgqF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nhRCc14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E6NRf4R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3NInx1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V3lnyl7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6aPq1f7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6Swib9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mlvvJwX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Xs7pIy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB1AMeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pPAQcAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jjV1n8U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XanSTFKCustomer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isMlkK3 Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ksXR7o1 Customer</t>
+  </si>
+  <si>
     <t xml:space="preserve">WvvPpiG</t>
   </si>
   <si>
-    <t xml:space="preserve">1234567890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">used</t>
-  </si>
-  <si>
     <t xml:space="preserve">CoqaXOD</t>
   </si>
   <si>
@@ -64,9 +220,6 @@
     <t xml:space="preserve">lA4cCsR</t>
   </si>
   <si>
-    <t xml:space="preserve">unused</t>
-  </si>
-  <si>
     <t xml:space="preserve">q0zwGrb</t>
   </si>
   <si>
@@ -82,6 +235,12 @@
     <t xml:space="preserve">T2uiDUi</t>
   </si>
   <si>
+    <t xml:space="preserve">inyh7Bv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FztzCiB</t>
+  </si>
+  <si>
     <t xml:space="preserve">2cz9A0O</t>
   </si>
   <si>
@@ -91,9 +250,15 @@
     <t xml:space="preserve">LSeT31B</t>
   </si>
   <si>
+    <t xml:space="preserve">NMxoKAa</t>
+  </si>
+  <si>
     <t xml:space="preserve">BsAnlZn</t>
   </si>
   <si>
+    <t xml:space="preserve">end user</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kb6BrnL</t>
   </si>
   <si>
@@ -109,6 +274,9 @@
     <t xml:space="preserve">ozUVSUS Customer</t>
   </si>
   <si>
+    <t xml:space="preserve">device</t>
+  </si>
+  <si>
     <t xml:space="preserve">777766668888333</t>
   </si>
   <si>
@@ -118,106 +286,7 @@
     <t xml:space="preserve">358608538029457</t>
   </si>
   <si>
-    <t xml:space="preserve">I2duawu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhi1hlr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StaticPass@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reseller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ig26GfY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k8BytpD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reseller user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kx0h9PW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uCOwwTh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aiY9k5x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TKLddPU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPL9tVN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5uqGbei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kp8Tw5Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retailer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JRxj2A3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0HWR4LR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">616lw2n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EmdUgqF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nhRCc14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E6NRf4R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3NInx1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V3lnyl7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6aPq1f7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6Swib9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mlvvJwX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3Xs7pIy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB1AMeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pPAQcAF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jjV1n8U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XanSTFKCustomer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isMlkK3 Customer</t>
+    <t>used</t>
   </si>
 </sst>
 </file>
@@ -324,11 +393,11 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -400,13 +469,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -455,72 +524,6 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -542,10 +545,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -565,7 +568,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -576,7 +579,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -587,7 +590,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -614,11 +617,11 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -638,7 +641,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -649,7 +652,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -660,13 +663,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -685,13 +688,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -711,7 +714,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -722,24 +725,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -758,13 +750,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -778,53 +770,25 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -843,17 +807,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -862,59 +826,59 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1234567890</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1234567890</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -923,12 +887,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -937,110 +901,110 @@
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1234567890</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -1049,204 +1013,544 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>12</v>
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first commit env independent and prod env access
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/smf.xlsx
+++ b/src/test/resources/testdata/smf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="98">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -52,6 +52,12 @@
     <t xml:space="preserve">aYAIx2R</t>
   </si>
   <si>
+    <t xml:space="preserve">3uTmUYQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jzUFeEe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pl0DFDw</t>
   </si>
   <si>
@@ -61,6 +67,12 @@
     <t xml:space="preserve">8BubxM9</t>
   </si>
   <si>
+    <t xml:space="preserve">wImtQY7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEalJRK</t>
+  </si>
+  <si>
     <t xml:space="preserve">puD4YmL</t>
   </si>
   <si>
@@ -70,6 +82,12 @@
     <t xml:space="preserve">7WNdd8C</t>
   </si>
   <si>
+    <t xml:space="preserve">Qq6NE2j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a6uPXeA</t>
+  </si>
+  <si>
     <t xml:space="preserve">8gvq2JN</t>
   </si>
   <si>
@@ -79,21 +97,39 @@
     <t xml:space="preserve">MFEVT8s</t>
   </si>
   <si>
+    <t xml:space="preserve">YKfT4Gd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v9UFPqB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptOj0zS Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xPocWW Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GuKLYnC Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hgfu4vW Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">352915305692302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">354150266351986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">353862360615938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">357789750362728</t>
+  </si>
+  <si>
     <t xml:space="preserve">unused</t>
   </si>
   <si>
-    <t xml:space="preserve">ptOj0zS Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xPocWW Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">352915305692302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">354150266351986</t>
-  </si>
-  <si>
     <t xml:space="preserve">I2duawu</t>
   </si>
   <si>
@@ -284,9 +320,6 @@
   </si>
   <si>
     <t xml:space="preserve">358608538029457</t>
-  </si>
-  <si>
-    <t>used</t>
   </si>
 </sst>
 </file>
@@ -391,13 +424,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -450,6 +483,28 @@
         <v>4</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -469,13 +524,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -495,7 +550,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -506,7 +561,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -517,12 +572,34 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -542,13 +619,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -568,7 +645,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -579,7 +656,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -590,12 +667,34 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -615,13 +714,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -641,7 +740,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -652,7 +751,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -663,13 +762,35 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -688,13 +809,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -714,7 +835,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -725,13 +846,35 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -750,13 +893,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -771,24 +914,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -813,11 +978,11 @@
       <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -826,59 +991,59 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1234567890</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1234567890</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -887,12 +1052,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -901,110 +1066,110 @@
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1234567890</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -1013,220 +1178,220 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>4</v>
@@ -1235,12 +1400,12 @@
         <v>5</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
@@ -1251,7 +1416,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
@@ -1262,7 +1427,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>4</v>
@@ -1271,12 +1436,12 @@
         <v>5</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>4</v>
@@ -1287,7 +1452,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>4</v>
@@ -1298,7 +1463,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
@@ -1309,7 +1474,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>4</v>
@@ -1320,7 +1485,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>4</v>
@@ -1331,7 +1496,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>4</v>
@@ -1342,7 +1507,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>4</v>
@@ -1353,7 +1518,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>4</v>
@@ -1364,7 +1529,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>4</v>
@@ -1375,18 +1540,18 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
@@ -1395,12 +1560,12 @@
         <v>5</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>4</v>
@@ -1411,7 +1576,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>4</v>
@@ -1422,7 +1587,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
@@ -1433,7 +1598,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
@@ -1442,12 +1607,12 @@
         <v>5</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
@@ -1458,7 +1623,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>4</v>
@@ -1469,7 +1634,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>4</v>
@@ -1480,7 +1645,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
@@ -1491,7 +1656,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
@@ -1508,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1687,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>4</v>
@@ -1533,7 +1698,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
@@ -1544,7 +1709,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>

</xml_diff>